<commit_message>
start adding generic solution using elements names insted fixed location
</commit_message>
<xml_diff>
--- a/Students_Grades.xlsx
+++ b/Students_Grades.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Students_Grades" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -461,19 +461,18 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['33.333333333333336/100', '100.0/100']</t>
+          <t>33.33 / 100.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>student_display_name_with_only_last_name: failed
-student_display_name_with_only_first_name: succeeded
 student_display_full_name: failed</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>33.333333333333336/100.0</t>
+          <t>33.33/100.0</t>
         </is>
       </c>
     </row>
@@ -483,26 +482,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['33.333333333333336/100', '100.0/100']</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>student_display_name_with_only_last_name: failed
-student_display_name_with_only_first_name: succeeded
-student_display_full_name: failed
-student_display_name_with_only_last_name: succeeded
-student_display_name_with_only_first_name: succeeded
-student_display_full_name: succeeded</t>
-        </is>
-      </c>
+          <t>100.0 / 100.0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>133.33333333333334/200.0</t>
+          <t>100.0/100.0</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
seperating lecturer config and student solution running
</commit_message>
<xml_diff>
--- a/Students_Grades.xlsx
+++ b/Students_Grades.xlsx
@@ -461,18 +461,18 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>33.33 / 100.0</t>
+          <t>0.0 / 100.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>student_display_name_with_only_last_name: failed
-student_display_full_name: failed</t>
+          <t xml:space="preserve">
+</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>33.33/100.0</t>
+          <t>0.0/100.0</t>
         </is>
       </c>
     </row>
@@ -482,13 +482,18 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>100.0 / 100.0</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
+          <t>0.0 / 100.0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>100.0/100.0</t>
+          <t>0.0/100.0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
exe 1 90% working
</commit_message>
<xml_diff>
--- a/Students_Grades.xlsx
+++ b/Students_Grades.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Students_Grades" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -461,18 +461,18 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.0 / 100.0</t>
+          <t>33.33 / 100.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-</t>
+          <t>display_name_with_only_last_name: failed
+display_full_name: failed</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.0/100.0</t>
+          <t>33.33/100.0</t>
         </is>
       </c>
     </row>
@@ -482,22 +482,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.0 / 100.0</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-</t>
-        </is>
-      </c>
+          <t>100.0 / 100.0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.0/100.0</t>
+          <t>100.0/100.0</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finish student tests for hw3
</commit_message>
<xml_diff>
--- a/Students_Grades.xlsx
+++ b/Students_Grades.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,15 +441,55 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>display_name_score</t>
+          <t>is_list_ordered_score</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>display_name_review</t>
+          <t>is_list_ordered_review</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>picking_right_pair_score</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>picking_right_pair_review</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>picking_wrong_pair_score</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>picking_wrong_pair_review</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>picking_zero_pair_score</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>picking_zero_pair_review</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>picking_only_one_element_score</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>picking_only_one_element_review</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>final_score</t>
         </is>
@@ -461,18 +501,48 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>33.33 / 100.0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>display_name_with_only_last_name: failed
-display_full_name: failed</t>
-        </is>
-      </c>
+          <t>20.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>33.33/100.0</t>
+          <t>4.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>bruce_wayne_and_wayne_enterprises: failed
+clark_kent_and_daily_planet: failed
+peter_parker_and_daily_bugle: failed
+willie_wonka_and_chocolate_factory: failed</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>bruce_wayne_and_chocolate_factory: failed</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>20.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>20.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>64.0/100.0</t>
         </is>
       </c>
     </row>
@@ -482,11 +552,35 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>100.0 / 100.0</t>
+          <t>20.0 / 20.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
+        <is>
+          <t>20.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>20.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>20.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>20.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
         <is>
           <t>100.0/100.0</t>
         </is>

</xml_diff>

<commit_message>
revamp report headers names and reviews names with replacing "_" with " "
</commit_message>
<xml_diff>
--- a/Students_Grades.xlsx
+++ b/Students_Grades.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,20 +436,60 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>student_ids</t>
+          <t>student ids</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>display_name_score</t>
+          <t>is list ordered score</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>display_name_review</t>
+          <t>is list ordered review</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>picking right pair score</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>picking right pair review</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>picking wrong pair score</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>picking wrong pair review</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>picking zero pair score</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>picking zero pair review</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>picking only one element score</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>picking only one element review</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>final_score</t>
         </is>
@@ -461,18 +501,48 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>33.33 / 100.0</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>display_name_with_only_last_name: failed
-display_full_name: failed</t>
-        </is>
-      </c>
+          <t>20.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>33.33/100.0</t>
+          <t>4.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>bruce wayne and wayne enterprises: failed
+clark kent and daily planet: failed
+peter parker and daily bugle: failed
+willie wonka and chocolate factory: failed</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>bruce wayne and chocolate factory: failed</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>20.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>20.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>64.0/100.0</t>
         </is>
       </c>
     </row>
@@ -482,11 +552,35 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>100.0 / 100.0</t>
+          <t>20.0 / 20.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
+        <is>
+          <t>20.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>20.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>20.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>20.0 / 20.0</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
         <is>
           <t>100.0/100.0</t>
         </is>

</xml_diff>

<commit_message>
creating full app imgs for lecturer and student
</commit_message>
<xml_diff>
--- a/Students_Grades.xlsx
+++ b/Students_Grades.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,15 +441,30 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>bahamas review</t>
+          <t>is list ordered review</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>zambia review</t>
+          <t>picking right pair review</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>picking wrong pair review</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>picking zero pair review</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>picking only one element review</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>final score</t>
         </is>
@@ -461,63 +476,78 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>score:0.0 / 50.0
-bahamas continent: failed
-bahamas population: failed
-bahamas area: failed</t>
+          <t xml:space="preserve">score:20.0 / 20.0
+</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>score:0.0 / 50.0
-zambia continent: failed
-zambia population: failed
-zambia area: failed</t>
+          <t>score:4.0 / 20.0
+bruce wayne and wayne enterprises: failed
+clark kent and daily planet: failed
+peter parker and daily bugle: failed
+willie wonka and chocolate factory: failed</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.0/100.0</t>
+          <t>score:0.0 / 20.0
+bruce wayne and chocolate factory: failed</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">score:20.0 / 20.0
+</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">score:20.0 / 20.0
+</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>64.0/100.0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>302967899</v>
+        <v>308418367</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>score: 0/0, could not find gui elements</t>
+          <t xml:space="preserve">score:20.0 / 20.0
+</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>score: 0/0, could not find gui elements</t>
+          <t xml:space="preserve">score:20.0 / 20.0
+</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.0/100.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>308418367</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">score:50.0 / 50.0
-</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">score:50.0 / 50.0
-</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
+          <t xml:space="preserve">score:20.0 / 20.0
+</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">score:20.0 / 20.0
+</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">score:20.0 / 20.0
+</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>100.0/100.0</t>
         </is>

</xml_diff>

<commit_message>
finished project just need to clean a bit code / doco
</commit_message>
<xml_diff>
--- a/Students_Grades.xlsx
+++ b/Students_Grades.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,27 +441,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>is list ordered review</t>
+          <t>afghanistan review</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>picking right pair review</t>
+          <t>albania review</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>picking wrong pair review</t>
+          <t>Azerbaijan review</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>picking zero pair review</t>
+          <t>bahamas review</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>picking only one element review</t>
+          <t>zambia review</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -476,78 +476,120 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">score:20.0 / 20.0
-</t>
+          <t>score:0.0 / 20.0
+afghanistan continent: failed
+afghanistan population: failed
+afghanistan area: failed</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>score:4.0 / 20.0
-bruce wayne and wayne enterprises: failed
-clark kent and daily planet: failed
-peter parker and daily bugle: failed
-willie wonka and chocolate factory: failed</t>
+          <t>score:0.0 / 20.0
+albania continent: failed
+albania population: failed
+albania area: failed</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>score:0.0 / 20.0
-bruce wayne and chocolate factory: failed</t>
+Azerbaijan continent: failed
+Azerbaijan population: failed
+Azerbaijan area: failed</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">score:20.0 / 20.0
-</t>
+          <t>score:0.0 / 20.0
+bahamas continent: failed
+bahamas population: failed
+bahamas area: failed</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">score:20.0 / 20.0
-</t>
+          <t>score:0.0 / 20.0
+zambia continent: failed
+zambia population: failed
+zambia area: failed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>64.0/100.0</t>
+          <t>0.0/100.0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>302967899</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>score: 0/0, could not find gui elements</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>score: 0/0, could not find gui elements</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>score: 0/0, could not find gui elements</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>score: 0/0, could not find gui elements</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>score: 0/0, could not find gui elements</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.0/100.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>308418367</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t xml:space="preserve">score:20.0 / 20.0
 </t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t xml:space="preserve">score:20.0 / 20.0
 </t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t xml:space="preserve">score:20.0 / 20.0
 </t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t xml:space="preserve">score:20.0 / 20.0
 </t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t xml:space="preserve">score:20.0 / 20.0
 </t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>100.0/100.0</t>
         </is>

</xml_diff>

<commit_message>
final refactor into modules
</commit_message>
<xml_diff>
--- a/Students_Grades.xlsx
+++ b/Students_Grades.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,10 +441,30 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>display name review</t>
+          <t>is list ordered review</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>picking right pair review</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>picking wrong pair review</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>picking zero pair review</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>picking only one element review</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>final score</t>
         </is>
@@ -456,14 +476,40 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>score:33.33 / 100.0
-display name with only last name: failed
-display full name: failed</t>
+          <t xml:space="preserve">score:20.0 / 20.0
+</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>33.33/100.0</t>
+          <t>score:4.0 / 20.0
+bruce wayne and wayne enterprises: failed
+clark kent and daily planet: failed
+peter parker and daily bugle: failed
+willie wonka and chocolate factory: failed</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>score:0.0 / 20.0
+bruce wayne and chocolate factory: failed</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">score:20.0 / 20.0
+</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">score:20.0 / 20.0
+</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>64.0/100.0</t>
         </is>
       </c>
     </row>
@@ -473,11 +519,35 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">score:100.0 / 100.0
+          <t xml:space="preserve">score:20.0 / 20.0
 </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">score:20.0 / 20.0
+</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">score:20.0 / 20.0
+</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">score:20.0 / 20.0
+</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">score:20.0 / 20.0
+</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>100.0/100.0</t>
         </is>

</xml_diff>